<commit_message>
Revisada conectividad entre fragment y DAO. Falta conectividad activity-fragment
</commit_message>
<xml_diff>
--- a/Esquema de Base de Datos.xlsx
+++ b/Esquema de Base de Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_ROOT\Academia\INACAP\Semestre 4\Android\Proyecto Semestral\ProyectoADBJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C565A64C-078E-44B1-A615-E769659D61CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7682DAC-0AB2-433B-9822-FD8F6C104966}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="16440" activeTab="1" xr2:uid="{D5718C2F-95B8-4006-960E-80CBF4D4217A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="70">
   <si>
     <t>USUARIOS</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>id_clase</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -435,6 +438,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,11 +461,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,21 +794,21 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="E2" s="14" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="E2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="I2" s="14" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -872,11 +877,11 @@
         <v>14</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -947,21 +952,21 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="E12" s="14" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="E12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="I12" s="17" t="s">
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="I12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1046,18 +1051,18 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1094,11 +1099,11 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
       <c r="I22" s="5"/>
       <c r="J22" s="10"/>
       <c r="K22" s="5"/>
@@ -1138,16 +1143,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E17:G17"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1155,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E4DCB9-04C1-48E2-A08F-0FE2FDF9E7C7}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,15 +1177,15 @@
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="22"/>
+    <col min="17" max="17" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1199,15 +1204,15 @@
       <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21"/>
       <c r="P1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="R1" s="12" t="s">
@@ -1259,13 +1264,13 @@
       <c r="P2" s="12">
         <v>1</v>
       </c>
-      <c r="Q2" s="21">
+      <c r="Q2" s="15">
         <v>43749</v>
       </c>
-      <c r="R2" s="23">
+      <c r="R2" s="17">
         <v>16</v>
       </c>
-      <c r="S2" s="23">
+      <c r="S2" s="17">
         <v>20</v>
       </c>
       <c r="T2" s="12">
@@ -1278,7 +1283,7 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="12">
@@ -1307,13 +1312,13 @@
       <c r="P3" s="12">
         <v>2</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="15">
         <v>43750</v>
       </c>
-      <c r="R3" s="23">
+      <c r="R3" s="17">
         <v>17</v>
       </c>
-      <c r="S3" s="23">
+      <c r="S3" s="17">
         <v>21</v>
       </c>
       <c r="T3" s="12">
@@ -1355,13 +1360,13 @@
       <c r="P4" s="12">
         <v>3</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="15">
         <v>43750</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="17">
         <v>16</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="17">
         <v>20</v>
       </c>
       <c r="T4" s="12">
@@ -1407,13 +1412,13 @@
       <c r="P5" s="12">
         <v>4</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="15">
         <v>43751</v>
       </c>
-      <c r="R5" s="23">
+      <c r="R5" s="17">
         <v>17</v>
       </c>
-      <c r="S5" s="23">
+      <c r="S5" s="17">
         <v>21</v>
       </c>
       <c r="T5" s="12">
@@ -1424,7 +1429,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
@@ -1461,13 +1468,13 @@
       <c r="P6" s="12">
         <v>5</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="15">
         <v>43752</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="17">
         <v>16</v>
       </c>
-      <c r="S6" s="23">
+      <c r="S6" s="17">
         <v>20</v>
       </c>
       <c r="T6" s="12">
@@ -1478,11 +1485,6 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1495,13 +1497,13 @@
       <c r="P7" s="12">
         <v>6</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="15">
         <v>43753</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="17">
         <v>17</v>
       </c>
-      <c r="S7" s="23">
+      <c r="S7" s="17">
         <v>21</v>
       </c>
       <c r="T7" s="12">
@@ -1511,371 +1513,392 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="E10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="E12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="E11" s="12">
-        <v>1</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="E12" s="12">
-        <v>2</v>
-      </c>
-      <c r="F12" s="12" t="s">
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="E14" s="12">
+        <v>2</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="E15" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="E17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="E16" s="12">
-        <v>1</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G18" s="12">
         <v>100000</v>
       </c>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="E17" s="12">
-        <v>2</v>
-      </c>
-      <c r="F17" s="12" t="s">
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="E19" s="12">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G19" s="12">
         <v>80000</v>
       </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="E18" s="12">
+      <c r="C20" s="6"/>
+      <c r="E20" s="12">
         <v>3</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G20" s="12">
         <v>50000</v>
       </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="11" t="s">
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="E19" s="12">
+      <c r="C21" s="9"/>
+      <c r="E21" s="12">
         <v>4</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G21" s="12">
         <v>30000</v>
       </c>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="E20" s="12">
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="E22" s="12">
         <v>5</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G22" s="12">
         <v>15000</v>
       </c>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="E22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="12" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="E24" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H24" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="12">
-        <v>1</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="E24" s="12">
-        <v>2</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="12">
-        <v>2</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="E26" s="12">
+        <v>2</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="12">
+        <v>2</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E27" s="12">
         <v>3</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="12">
-        <v>2</v>
-      </c>
-      <c r="H25" s="12" t="s">
+      <c r="G27" s="12">
+        <v>2</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="s">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="E26" s="12">
+      <c r="C28" s="9"/>
+      <c r="E28" s="12">
         <v>4</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F28" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="12">
-        <v>2</v>
-      </c>
-      <c r="H26" s="12" t="s">
+      <c r="G28" s="12">
+        <v>2</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="12">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="12">
         <v>5</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="12">
-        <v>2</v>
-      </c>
-      <c r="H27" s="12" t="s">
+      <c r="G29" s="12">
+        <v>2</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
-      <c r="E29" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="E31" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="E30" s="12">
-        <v>1</v>
-      </c>
-      <c r="F30" s="12" t="s">
+      <c r="B32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="E32" s="12">
+        <v>1</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="E31" s="12">
-        <v>2</v>
-      </c>
-      <c r="F31" s="12" t="s">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="B37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="G38" s="18"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>